<commit_message>
added checks for RGT in download report
</commit_message>
<xml_diff>
--- a/compat/tablesSchema.1.1.3.xlsx
+++ b/compat/tablesSchema.1.1.3.xlsx
@@ -4542,10 +4542,10 @@
   <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O9" sqref="O9"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6479,10 +6479,10 @@
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M3" sqref="M3"/>
+      <selection pane="bottomRight" activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>